<commit_message>
minor update before release
</commit_message>
<xml_diff>
--- a/CPMMS_software/excel file template/import_excel_data_template.xlsx
+++ b/CPMMS_software/excel file template/import_excel_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CPMMS\CPMMS_software\excel file template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AB4327-CBD5-4871-A12D-8BCC7D1057C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA69117-AB23-44FB-99C2-3200810F754B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0F94CEF-9A0C-452D-A493-8F7576F7E439}"/>
+    <workbookView xWindow="450" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{B0F94CEF-9A0C-452D-A493-8F7576F7E439}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>BARCODE ID</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>IN STOCK</t>
+  </si>
+  <si>
+    <t>ITEM CATEGORY</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC54E126-E160-4915-8942-81A7CF1036D1}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,9 +423,10 @@
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -435,6 +439,9 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>